<commit_message>
latest SustSol bills paid ;-)
</commit_message>
<xml_diff>
--- a/Planning/overview_planning_25_expire_sustsol.xlsx
+++ b/Planning/overview_planning_25_expire_sustsol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernd/financials/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FAD4A5-E773-0646-BE19-3F3BD37DBC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20293C7B-53A9-1049-8F66-74D8F5DDB302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="620" windowWidth="30080" windowHeight="33220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27680" yWindow="620" windowWidth="32480" windowHeight="33220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview25" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1094,6 +1094,8 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent 1 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1304,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMC173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView topLeftCell="A74" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.5" customHeight="1"/>
@@ -2855,6 +2857,11 @@
         <v>164</v>
       </c>
       <c r="H95" s="89"/>
+      <c r="I95" s="111"/>
+      <c r="J95" s="111"/>
+      <c r="K95" s="111"/>
+      <c r="L95" s="112"/>
+      <c r="M95" s="112"/>
       <c r="N95" s="92"/>
     </row>
     <row r="96" spans="2:14" ht="15">
@@ -2862,7 +2869,7 @@
         <v>45901</v>
       </c>
       <c r="E96" s="4">
-        <v>-900</v>
+        <v>-1060</v>
       </c>
       <c r="F96" s="27" t="s">
         <v>80</v>
@@ -2870,50 +2877,58 @@
       <c r="H96" s="90">
         <v>45902</v>
       </c>
-      <c r="J96" s="4">
+      <c r="I96" s="111"/>
+      <c r="J96" s="111">
         <v>18000</v>
       </c>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
+      <c r="K96" s="111"/>
+      <c r="L96" s="111"/>
+      <c r="M96" s="111"/>
       <c r="N96" s="92" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="97" spans="2:14" ht="15">
-      <c r="B97" s="20">
-        <v>45894</v>
-      </c>
-      <c r="C97" s="18">
-        <f>SUM(C91:E96)</f>
-        <v>29450.520000000004</v>
-      </c>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="107"/>
+      <c r="B97" s="26">
+        <v>45904</v>
+      </c>
+      <c r="D97" s="4">
+        <v>14000</v>
+      </c>
+      <c r="F97" s="92" t="s">
+        <v>8</v>
+      </c>
       <c r="H97" s="90">
         <v>45904</v>
       </c>
-      <c r="L97" s="4">
-        <v>-12000</v>
-      </c>
-      <c r="M97" s="4"/>
+      <c r="I97" s="111"/>
+      <c r="J97" s="111"/>
+      <c r="K97" s="111"/>
+      <c r="L97" s="111">
+        <v>-14000</v>
+      </c>
+      <c r="M97" s="111"/>
       <c r="N97" s="92" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="98" spans="2:14" ht="15">
-      <c r="B98" s="26">
-        <v>45905</v>
-      </c>
-      <c r="D98" s="4">
-        <v>12000</v>
-      </c>
-      <c r="F98" s="92" t="s">
-        <v>8</v>
-      </c>
-      <c r="H98" s="90"/>
-      <c r="L98" s="4"/>
-      <c r="M98" s="4"/>
+      <c r="B98" s="20">
+        <v>45894</v>
+      </c>
+      <c r="C98" s="18">
+        <f>SUM(C91:E97)</f>
+        <v>43290.520000000004</v>
+      </c>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="107"/>
+      <c r="H98" s="89"/>
+      <c r="I98" s="111"/>
+      <c r="J98" s="111"/>
+      <c r="K98" s="111"/>
+      <c r="L98" s="112"/>
+      <c r="M98" s="112"/>
       <c r="N98" s="92"/>
     </row>
     <row r="99" spans="2:14" ht="15">
@@ -2945,7 +2960,7 @@
       </c>
       <c r="E100" s="4">
         <f>-CostBlocks25!$L$15-E67-E80/2-E81-E77-E85-E79-E84-E86-E88/2-E96/2</f>
-        <v>-1545.3200000000002</v>
+        <v>-1465.3200000000002</v>
       </c>
       <c r="F100" s="92" t="s">
         <v>149</v>
@@ -2959,7 +2974,7 @@
       </c>
       <c r="E101" s="4">
         <f>-3*CostBlocks25!$C$19-E80/2-E88/2-E96/2</f>
-        <v>-715</v>
+        <v>-635</v>
       </c>
       <c r="F101" s="92" t="s">
         <v>83</v>
@@ -2973,8 +2988,8 @@
         <v>45931</v>
       </c>
       <c r="C102" s="18">
-        <f>SUM(C97:E101)</f>
-        <v>39415.200000000004</v>
+        <f>SUM(C98:E101)</f>
+        <v>41415.200000000004</v>
       </c>
       <c r="D102" s="18"/>
       <c r="E102" s="18"/>
@@ -2984,7 +2999,7 @@
       </c>
       <c r="I102" s="18">
         <f>SUM(I83:M101)</f>
-        <v>5864.8499999999985</v>
+        <v>3864.8499999999985</v>
       </c>
       <c r="J102" s="18"/>
       <c r="K102" s="18"/>
@@ -3024,7 +3039,7 @@
       </c>
       <c r="H104" s="38"/>
       <c r="L104" s="4">
-        <v>-8000</v>
+        <v>-7000</v>
       </c>
     </row>
     <row r="105" spans="2:14" ht="15">
@@ -3121,7 +3136,7 @@
         <v>46022</v>
       </c>
       <c r="D109" s="4">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="F109" s="92" t="s">
         <v>8</v>
@@ -3132,7 +3147,7 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4">
         <f>(L112*0.05)*1.02-M48-M86</f>
-        <v>-989.77999999999986</v>
+        <v>-1040.7799999999997</v>
       </c>
       <c r="N109" s="92" t="s">
         <v>87</v>
@@ -3144,7 +3159,7 @@
       </c>
       <c r="C110" s="31">
         <f>SUM(C102:E109)</f>
-        <v>41313.700000000004</v>
+        <v>42313.700000000004</v>
       </c>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
@@ -3154,7 +3169,7 @@
       </c>
       <c r="I110" s="31">
         <f>SUM(I102:M109)</f>
-        <v>1141.7279999999982</v>
+        <v>90.727999999998246</v>
       </c>
       <c r="J110" s="31"/>
       <c r="K110" s="31"/>
@@ -3174,7 +3189,7 @@
       </c>
       <c r="C112" s="36">
         <f>C110+P110+I110</f>
-        <v>42455.428</v>
+        <v>42404.428</v>
       </c>
       <c r="D112" s="36"/>
       <c r="E112" s="36"/>
@@ -3192,11 +3207,11 @@
       </c>
       <c r="L112" s="37">
         <f t="shared" ref="L112:M112" si="0">SUM(L7:L109)</f>
-        <v>-38500</v>
+        <v>-39500</v>
       </c>
       <c r="M112" s="37">
         <f t="shared" si="0"/>
-        <v>-12607.102000000001</v>
+        <v>-12658.101999999999</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="15">
@@ -3450,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:O53"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="13.5" customHeight="1"/>

</xml_diff>